<commit_message>
Created new Test Case and Test Data for IWP 3.0.
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/VRelay30PayNowCC.xlsx
+++ b/KatalonData/IWPTestData/VRelay30PayNowCC.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2495D291-9D00-4BC2-B9B3-3F7377033201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E82266F-CED3-4163-B816-6932CFBEE60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{19E085DA-5ADF-4B16-9D78-B410FD3FCE3D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{19E085DA-5ADF-4B16-9D78-B410FD3FCE3D}"/>
   </bookViews>
   <sheets>
     <sheet name="PayNowCC" sheetId="1" r:id="rId1"/>
-    <sheet name="MissingCC" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
+    <sheet name="PayNowCCSCF" sheetId="5" r:id="rId2"/>
+    <sheet name="PayNowCCDCF" sheetId="6" r:id="rId3"/>
+    <sheet name="DCFVerbiage" sheetId="8" r:id="rId4"/>
+    <sheet name="MissingCC" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId6"/>
+    <sheet name="SCFVerbiage" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="154">
   <si>
     <t>Notes</t>
   </si>
@@ -429,6 +433,75 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>6510000000000216</t>
+  </si>
+  <si>
+    <t>374245002771003</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>650</t>
+  </si>
+  <si>
+    <t>651</t>
+  </si>
+  <si>
+    <t>Verify Single CF Verbiage</t>
+  </si>
+  <si>
+    <t>Verify Dual CF Verbiage</t>
+  </si>
+  <si>
+    <t>Wed Jun 14 19:38:31 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jun 14 19:39:26 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jun 14 19:40:16 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jun 14 19:41:07 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jun 14 19:41:58 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jun 14 19:42:59 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jun 14 19:43:59 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jun 14 19:45:00 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jun 14 20:10:26 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jun 14 20:11:31 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jun 14 20:12:33 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Jun 14 20:13:34 EDT 2023</t>
   </si>
 </sst>
 </file>
@@ -812,189 +885,264 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4684B99E-74C7-4C50-809D-02154653C064}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z2" sqref="Z2"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="1"/>
-    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="1" customWidth="1"/>
-    <col min="11" max="15" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="23" style="1" customWidth="1"/>
-    <col min="19" max="19" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="15.7109375" style="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" collapsed="1"/>
+    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="16384" width="15.7109375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="Z2" s="2"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="AB2" s="2"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="R3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="W3" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="W5" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1009,6 +1157,711 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE14908-B016-4D5E-AEA7-D54DB9070BC6}">
+  <dimension ref="A1:AB5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" collapsed="1"/>
+    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="16384" width="15.7109375" style="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB2" s="2"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822FCC47-1993-44A8-9BE0-581A41644C90}">
+  <dimension ref="A1:AB5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" collapsed="1"/>
+    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="16384" width="15.7109375" style="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB2" s="2"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0550F98D-701F-463B-8524-B8E5F73F2D8E}">
+  <dimension ref="A1:AB5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" collapsed="1"/>
+    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="16384" width="15.7109375" style="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB2" s="2"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+      <c r="B3"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="B5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FB57A2-D7E3-4332-BF3A-D9FD91EC8308}">
   <dimension ref="A1:AX2"/>
   <sheetViews>
@@ -1018,44 +1871,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.7109375" style="1"/>
-    <col min="30" max="30" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="39" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.7109375" style="1" customWidth="1"/>
-    <col min="42" max="42" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="46" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="48" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="16384" width="15.7109375" style="1"/>
+    <col min="1" max="1" width="49.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="5.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="23" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="15.7109375" style="1" collapsed="1"/>
+    <col min="30" max="30" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="33" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="39" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="46" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="16384" width="15.7109375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
@@ -1249,17 +2102,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6029C9A2-9E58-4FB9-972D-7B9E934718A7}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B15"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1312,11 +2165,13 @@
       <c r="A9" t="s">
         <v>114</v>
       </c>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>115</v>
       </c>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1344,6 +2199,16 @@
         <v>121</v>
       </c>
       <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>141</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1353,7 +2218,179 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0998B4B-1379-4C62-AAAC-69FB8C23F4B6}">
+  <dimension ref="A1:AB5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" collapsed="1"/>
+    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="16384" width="15.7109375" style="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB2" s="2"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+      <c r="B3"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="B5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CECF72-ED76-4A08-B368-44E780FE04C9}">
   <dimension ref="A1:AX4"/>
   <sheetViews>
@@ -1363,44 +2400,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.7109375" style="1"/>
-    <col min="30" max="30" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="39" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="17.7109375" style="1" customWidth="1"/>
-    <col min="42" max="42" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="46" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="48" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="16384" width="15.7109375" style="1"/>
+    <col min="1" max="1" width="38.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="5.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="23" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="15.7109375" style="1" collapsed="1"/>
+    <col min="30" max="30" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="33" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="39" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="46" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="16384" width="15.7109375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Error-OverAndUnderPay Test Case and Data.
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/VRelay30PayNowCC.xlsx
+++ b/KatalonData/IWPTestData/VRelay30PayNowCC.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB550D3-D775-46C5-AB30-8572791483D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF647BBB-F32B-4061-AC01-8DC6A39C3A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{19E085DA-5ADF-4B16-9D78-B410FD3FCE3D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="6" xr2:uid="{19E085DA-5ADF-4B16-9D78-B410FD3FCE3D}"/>
   </bookViews>
   <sheets>
     <sheet name="PayNowCC" sheetId="1" r:id="rId1"/>
     <sheet name="PayNowCCSCF" sheetId="5" r:id="rId2"/>
     <sheet name="PayNowCCDCF" sheetId="6" r:id="rId3"/>
     <sheet name="DCFVerbiage" sheetId="8" r:id="rId4"/>
-    <sheet name="MissingCC" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId6"/>
-    <sheet name="SCFVerbiage" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId8"/>
+    <sheet name="OverUnderPay" sheetId="9" r:id="rId5"/>
+    <sheet name="MissingCC" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId7"/>
+    <sheet name="SCFVerbiage" sheetId="7" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="164">
   <si>
     <t>Notes</t>
   </si>
@@ -502,6 +503,36 @@
   </si>
   <si>
     <t>Wed Jun 14 20:13:34 EDT 2023</t>
+  </si>
+  <si>
+    <t>2001.50</t>
+  </si>
+  <si>
+    <t>1.50</t>
+  </si>
+  <si>
+    <t>ErrMsg</t>
+  </si>
+  <si>
+    <t>Amount is greater than maximum</t>
+  </si>
+  <si>
+    <t>Amount is less than minimum</t>
+  </si>
+  <si>
+    <t>Thu Jun 22 16:38:42 EDT 2023</t>
+  </si>
+  <si>
+    <t>Thu Jun 22 16:39:24 EDT 2023</t>
+  </si>
+  <si>
+    <t>Personal Checking</t>
+  </si>
+  <si>
+    <t>Personal Savings</t>
+  </si>
+  <si>
+    <t>Corporate</t>
   </si>
 </sst>
 </file>
@@ -1695,7 +1726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0550F98D-701F-463B-8524-B8E5F73F2D8E}">
   <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1862,6 +1893,227 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30327A80-5D3D-4DEF-87CB-A4BDC28D6002}">
+  <dimension ref="A1:AC5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="1" collapsed="1"/>
+    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" collapsed="1"/>
+    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="24" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="26" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="28.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="16384" width="15.7109375" style="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="B5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FB57A2-D7E3-4332-BF3A-D9FD91EC8308}">
   <dimension ref="A1:AX2"/>
   <sheetViews>
@@ -2102,12 +2354,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6029C9A2-9E58-4FB9-972D-7B9E934718A7}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2210,6 +2462,21 @@
         <v>141</v>
       </c>
     </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
@@ -2218,7 +2485,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0998B4B-1379-4C62-AAAC-69FB8C23F4B6}">
   <dimension ref="A1:AB5"/>
   <sheetViews>
@@ -2390,12 +2657,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CECF72-ED76-4A08-B368-44E780FE04C9}">
   <dimension ref="A1:AX4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD4"/>
+      <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed the IWPSmokeTest Test Suite execution order.
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/VRelay30PayNowCC.xlsx
+++ b/KatalonData/IWPTestData/VRelay30PayNowCC.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4781A4-65A2-4972-A8CB-E8056A17F4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{EE4781A4-65A2-4972-A8CB-E8056A17F4B4}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="6" xr2:uid="{19E085DA-5ADF-4B16-9D78-B410FD3FCE3D}"/>
+    <workbookView activeTab="6" windowHeight="17640" windowWidth="29040" xWindow="-120" xr2:uid="{19E085DA-5ADF-4B16-9D78-B410FD3FCE3D}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="PayNowCC" sheetId="1" r:id="rId1"/>
-    <sheet name="PayNowCCSCF" sheetId="5" r:id="rId2"/>
-    <sheet name="PayNowCCDCF" sheetId="6" r:id="rId3"/>
-    <sheet name="DCFVerbiage" sheetId="8" r:id="rId4"/>
-    <sheet name="OverUnderPay" sheetId="9" r:id="rId5"/>
-    <sheet name="MissingCC" sheetId="4" r:id="rId6"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId7"/>
-    <sheet name="NoModifyAmount" sheetId="10" r:id="rId8"/>
-    <sheet name="NoOverPay" sheetId="11" r:id="rId9"/>
-    <sheet name="SCFVerbiage" sheetId="7" r:id="rId10"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId11"/>
+    <sheet name="PayNowCC" r:id="rId1" sheetId="1"/>
+    <sheet name="PayNowCCSCF" r:id="rId2" sheetId="5"/>
+    <sheet name="PayNowCCDCF" r:id="rId3" sheetId="6"/>
+    <sheet name="DCFVerbiage" r:id="rId4" sheetId="8"/>
+    <sheet name="OverUnderPay" r:id="rId5" sheetId="9"/>
+    <sheet name="MissingCC" r:id="rId6" sheetId="4"/>
+    <sheet name="Sheet2" r:id="rId7" sheetId="3"/>
+    <sheet name="NoModifyAmount" r:id="rId8" sheetId="10"/>
+    <sheet name="NoOverPay" r:id="rId9" sheetId="11"/>
+    <sheet name="SCFVerbiage" r:id="rId10" sheetId="7"/>
+    <sheet name="Sheet1" r:id="rId11" sheetId="2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="180">
   <si>
     <t>Notes</t>
   </si>
@@ -577,12 +577,19 @@
   </si>
   <si>
     <t>Yes Over Pay</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Fri Jul 07 18:08:03 EDT 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -637,21 +644,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -668,10 +675,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -706,7 +713,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -758,7 +765,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -869,21 +876,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -900,7 +907,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -952,46 +959,46 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4684B99E-74C7-4C50-809D-02154653C064}">
-  <dimension ref="A1:AB5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4684B99E-74C7-4C50-809D-02154653C064}">
+  <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C14" sqref="C14"/>
+      <pane activePane="topRight" state="frozen" topLeftCell="D1" xSplit="3"/>
+      <selection activeCell="C14" pane="topRight" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" collapsed="1"/>
-    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="16384" width="15.7109375" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" style="1" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="29" max="16384" style="1" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -1082,10 +1089,10 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>124</v>
@@ -1223,8 +1230,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1232,8 +1239,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0998B4B-1379-4C62-AAAC-69FB8C23F4B6}">
-  <dimension ref="A1:AB5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0998B4B-1379-4C62-AAAC-69FB8C23F4B6}">
+  <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T2" sqref="T2"/>
@@ -1241,29 +1248,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" collapsed="1"/>
-    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="16384" width="15.7109375" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" style="1" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="29" max="16384" style="1" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -1399,13 +1406,13 @@
       <c r="B5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CECF72-ED76-4A08-B368-44E780FE04C9}">
-  <dimension ref="A1:AX4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1CECF72-ED76-4A08-B368-44E780FE04C9}">
+  <dimension ref="A1:AY4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="Q42" sqref="Q42"/>
@@ -1413,44 +1420,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="23" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="15.7109375" style="1" collapsed="1"/>
-    <col min="30" max="30" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="33" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="39" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="46" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="16384" width="15.7109375" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="38.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="4.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="5.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="6.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="23.85546875" collapsed="true"/>
+    <col min="18" max="23" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="29" max="29" style="1" width="15.7109375" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="32" max="33" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="34" max="39" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="41" max="41" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="45" max="46" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="47" max="48" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="51" max="16384" style="1" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
@@ -1910,7 +1917,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1918,8 +1925,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE14908-B016-4D5E-AEA7-D54DB9070BC6}">
-  <dimension ref="A1:AB5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE14908-B016-4D5E-AEA7-D54DB9070BC6}">
+  <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -1927,29 +1934,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" collapsed="1"/>
-    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="16384" width="15.7109375" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" style="1" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="29" max="16384" style="1" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -2181,13 +2188,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822FCC47-1993-44A8-9BE0-581A41644C90}">
-  <dimension ref="A1:AB5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822FCC47-1993-44A8-9BE0-581A41644C90}">
+  <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -2195,29 +2202,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" collapsed="1"/>
-    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="16384" width="15.7109375" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" style="1" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="29" max="16384" style="1" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -2448,13 +2455,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0550F98D-701F-463B-8524-B8E5F73F2D8E}">
-  <dimension ref="A1:AB5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0550F98D-701F-463B-8524-B8E5F73F2D8E}">
+  <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -2462,29 +2469,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" collapsed="1"/>
-    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="16384" width="15.7109375" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" style="1" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="29" max="16384" style="1" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -2618,13 +2625,13 @@
       <c r="B5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30327A80-5D3D-4DEF-87CB-A4BDC28D6002}">
-  <dimension ref="A1:AC5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30327A80-5D3D-4DEF-87CB-A4BDC28D6002}">
+  <dimension ref="A1:AD5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AC3" sqref="AC3"/>
@@ -2632,30 +2639,30 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" collapsed="1"/>
-    <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.7109375" style="1" collapsed="1"/>
-    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="23" style="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="28.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="16384" width="15.7109375" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" style="1" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="1" width="28.140625" collapsed="true"/>
+    <col min="30" max="16384" style="1" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -2747,7 +2754,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -2839,13 +2846,13 @@
       <c r="B5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FB57A2-D7E3-4332-BF3A-D9FD91EC8308}">
-  <dimension ref="A1:AX2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19FB57A2-D7E3-4332-BF3A-D9FD91EC8308}">
+  <dimension ref="A1:AY2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AX6" sqref="AX6"/>
@@ -2853,44 +2860,44 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="6.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="23" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="6.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="15.7109375" style="1" collapsed="1"/>
-    <col min="30" max="30" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="33" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="39" width="7.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="46" width="7.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="16384" width="15.7109375" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="49.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="4.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="5.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="6.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="23.85546875" collapsed="true"/>
+    <col min="18" max="23" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="29" max="29" style="1" width="15.7109375" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="32" max="33" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="34" max="39" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="41" max="41" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="45" max="46" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="47" max="48" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="51" max="16384" style="1" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
@@ -3077,7 +3084,7 @@
       <c r="AX2" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3085,8 +3092,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6029C9A2-9E58-4FB9-972D-7B9E934718A7}">
-  <dimension ref="A1:B26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6029C9A2-9E58-4FB9-972D-7B9E934718A7}">
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -3094,7 +3101,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="56.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3243,7 +3250,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -3251,8 +3258,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F5F0A8-DFAA-493B-B07B-97C59CBB0D66}">
-  <dimension ref="A1:AB2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F5F0A8-DFAA-493B-B07B-97C59CBB0D66}">
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -3260,27 +3267,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="17" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="9" max="17" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -3366,7 +3373,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="45" r="2" s="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -3403,13 +3410,13 @@
       <c r="AB2" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133992E5-F2D4-42EB-B2FB-D66167060930}">
-  <dimension ref="A1:AB2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133992E5-F2D4-42EB-B2FB-D66167060930}">
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -3417,27 +3424,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="17" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="24" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="9" max="17" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -3523,7 +3530,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -3563,6 +3570,6 @@
       <c r="AB2" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Some RAD updates and added CreateAutoPay-CreditCard test case.
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/VRelay30PayNowCC.xlsx
+++ b/KatalonData/IWPTestData/VRelay30PayNowCC.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="183">
   <si>
     <t>Notes</t>
   </si>
@@ -583,6 +583,15 @@
   </si>
   <si>
     <t>Fri Jul 07 18:08:03 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 11 17:13:22 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 11 17:14:17 EDT 2023</t>
+  </si>
+  <si>
+    <t>Wed Oct 11 17:15:07 EDT 2023</t>
   </si>
 </sst>
 </file>
@@ -1089,10 +1098,10 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>124</v>
@@ -1128,7 +1137,7 @@
         <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>124</v>
@@ -1163,7 +1172,7 @@
         <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>124</v>

</xml_diff>

<commit_message>
Updated Test Data for Account Type.
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/VRelay30PayNowCC.xlsx
+++ b/KatalonData/IWPTestData/VRelay30PayNowCC.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="198">
   <si>
     <t>Notes</t>
   </si>
@@ -589,6 +589,54 @@
   </si>
   <si>
     <t>Thu May 16 13:57:03 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 14 22:43:32 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 14 22:44:38 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 14 22:45:34 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 14 22:46:33 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 14 22:47:30 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 14 22:48:36 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 14 22:53:09 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 14 22:54:32 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 14 22:56:03 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 14 22:57:43 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 14 23:00:48 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 14 23:01:32 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 14 23:05:47 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 14 23:29:09 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 14 23:38:01 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Aug 15 03:22:29 EDT 2024</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1146,7 @@
         <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>124</v>
@@ -1134,7 +1182,7 @@
         <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>124</v>
@@ -1169,7 +1217,7 @@
         <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>124</v>
@@ -1204,7 +1252,7 @@
         <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>124</v>
@@ -2056,7 +2104,7 @@
         <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>124</v>
@@ -2089,10 +2137,10 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>187</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>124</v>
@@ -2124,10 +2172,10 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>188</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>124</v>
@@ -2159,10 +2207,10 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>124</v>
@@ -2321,10 +2369,10 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>124</v>
@@ -2357,10 +2405,10 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>191</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>124</v>
@@ -2392,10 +2440,10 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>124</v>
@@ -2427,10 +2475,10 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>124</v>
@@ -2762,10 +2810,10 @@
     </row>
     <row ht="29.15" r="2" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
+        <v>195</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>111</v>
@@ -2804,10 +2852,10 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>112</v>
@@ -3381,10 +3429,10 @@
     </row>
     <row customFormat="1" ht="29.15" r="2" s="1" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>152</v>
@@ -3538,10 +3586,10 @@
     </row>
     <row customFormat="1" r="2" s="1" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>154</v>

</xml_diff>

<commit_message>
Updated VRelay 3.0 Test Cases.
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/VRelay30PayNowCC.xlsx
+++ b/KatalonData/IWPTestData/VRelay30PayNowCC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{343F8F64-B1BD-47B2-B0AE-8E7D353D1726}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{0CE3E5A1-26FC-4A67-A68D-A1ED38FB5808}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="7" windowHeight="21220" windowWidth="38620" xWindow="-110" xr2:uid="{19E085DA-5ADF-4B16-9D78-B410FD3FCE3D}" yWindow="-110"/>
+    <workbookView activeTab="2" windowHeight="13770" windowWidth="25860" xWindow="3045" xr2:uid="{19E085DA-5ADF-4B16-9D78-B410FD3FCE3D}" yWindow="1650"/>
   </bookViews>
   <sheets>
     <sheet name="PayNowCC" r:id="rId1" sheetId="1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="188">
   <si>
     <t>Notes</t>
   </si>
@@ -525,118 +525,88 @@
     <t>Yes Over Pay</t>
   </si>
   <si>
-    <t>Wed May 15 15:10:28 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed May 15 15:11:24 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed May 15 15:12:17 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed May 15 15:13:07 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed May 15 15:13:59 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed May 15 15:15:01 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed May 15 15:16:03 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed May 15 15:17:04 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed May 15 15:18:07 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed May 15 15:19:08 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed May 15 15:20:10 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed May 15 15:21:12 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed May 15 15:23:50 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed May 15 15:48:57 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed May 15 15:49:37 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed May 15 16:09:01 EDT 2024</t>
-  </si>
-  <si>
     <t>825</t>
   </si>
   <si>
     <t>824</t>
   </si>
   <si>
+    <t>Wed Aug 28 22:22:31 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 28 22:24:41 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 28 22:26:52 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 28 22:29:02 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 28 22:31:13 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 28 22:33:24 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 28 22:35:34 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 28 22:37:44 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 28 22:42:47 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 28 22:55:42 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 28 22:56:29 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 28 23:11:55 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Aug 29 17:56:34 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Aug 29 17:57:36 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Aug 29 17:58:34 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Aug 29 17:59:31 EDT 2024</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Thu May 16 13:51:56 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu May 16 13:53:09 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu May 16 13:57:03 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Aug 14 22:43:32 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Aug 14 22:44:38 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Aug 14 22:45:34 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Aug 14 22:46:33 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Aug 14 22:47:30 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Aug 14 22:48:36 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Aug 14 22:53:09 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Aug 14 22:54:32 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Aug 14 22:56:03 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Aug 14 22:57:43 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Aug 14 23:00:48 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Aug 14 23:01:32 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Aug 14 23:05:47 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Aug 14 23:29:09 EDT 2024</t>
-  </si>
-  <si>
-    <t>Wed Aug 14 23:38:01 EDT 2024</t>
-  </si>
-  <si>
-    <t>Thu Aug 15 03:22:29 EDT 2024</t>
+    <t>Thu Aug 29 20:16:47 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Aug 29 20:17:58 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Aug 29 20:19:07 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Aug 29 20:20:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Aug 29 20:25:15 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Aug 29 20:26:26 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Aug 29 20:27:34 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Aug 29 20:28:41 EDT 2024</t>
+  </si>
+  <si>
+    <t>Thu Aug 29 20:35:49 EDT 2024</t>
   </si>
 </sst>
 </file>
@@ -725,9 +695,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
@@ -765,7 +735,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
@@ -871,7 +841,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1013,7 +983,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office 2013 - 2022 Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1028,34 +998,34 @@
       <selection activeCell="C14" pane="topRight" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="15.69140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.3046875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.3046875" collapsed="true"/>
+    <col min="1" max="1" style="1" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.15234375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.3828125" collapsed="true"/>
-    <col min="7" max="7" style="1" width="15.69140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.3828125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.84375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.15234375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.69140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="13.3046875" collapsed="true"/>
-    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.84375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.84375" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="1" width="17.69140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" style="1" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
     <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.15234375" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.3828125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.15234375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
     <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
     <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="29" max="16384" style="1" width="15.69140625" collapsed="true"/>
+    <col min="29" max="16384" style="1" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -1141,12 +1111,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>124</v>
@@ -1177,12 +1147,12 @@
       </c>
       <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>124</v>
@@ -1212,12 +1182,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>124</v>
@@ -1247,12 +1217,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>124</v>
@@ -1300,34 +1270,34 @@
       <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="15.69140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.3046875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.3046875" collapsed="true"/>
+    <col min="1" max="1" style="1" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.15234375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.3828125" collapsed="true"/>
-    <col min="7" max="7" style="1" width="15.69140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.3828125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.84375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.15234375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.69140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="13.3046875" collapsed="true"/>
-    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.84375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.84375" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="1" width="17.69140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" style="1" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
     <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.15234375" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.3828125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.15234375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
     <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
     <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="29" max="16384" style="1" width="15.69140625" collapsed="true"/>
+    <col min="29" max="16384" style="1" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -1413,7 +1383,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>137</v>
       </c>
@@ -1447,15 +1417,15 @@
       </c>
       <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5"/>
     </row>
@@ -1472,49 +1442,49 @@
       <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="38.53515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="38.5703125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="4.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="8.15234375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="8.3046875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="6.84375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="13.84375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.3828125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="5.53515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="5.5703125" collapsed="true"/>
     <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="6.15234375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.69140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="23.84375" collapsed="true"/>
-    <col min="18" max="23" bestFit="true" customWidth="true" style="1" width="9.69140625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="1" width="9.84375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="6.84375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="9.69140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="10.69140625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="6.3828125" collapsed="true"/>
-    <col min="29" max="29" style="1" width="15.69140625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="10.3828125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="7.84375" collapsed="true"/>
-    <col min="32" max="33" bestFit="true" customWidth="true" style="1" width="9.69140625" collapsed="true"/>
-    <col min="34" max="39" bestFit="true" customWidth="true" style="1" width="7.84375" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" style="1" width="8.84375" collapsed="true"/>
-    <col min="41" max="41" customWidth="true" style="1" width="17.69140625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="17.3046875" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="8.15234375" collapsed="true"/>
-    <col min="45" max="46" bestFit="true" customWidth="true" style="1" width="7.3828125" collapsed="true"/>
-    <col min="47" max="48" bestFit="true" customWidth="true" style="1" width="9.15234375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="6.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="23.85546875" collapsed="true"/>
+    <col min="18" max="23" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="29" max="29" style="1" width="15.7109375" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="32" max="33" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="34" max="39" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="41" max="41" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="45" max="46" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="47" max="48" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
     <col min="49" max="49" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
     <col min="50" max="50" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="51" max="16384" style="1" width="15.69140625" collapsed="true"/>
+    <col min="51" max="16384" style="1" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1666,7 +1636,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>105</v>
       </c>
@@ -1750,7 +1720,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>106</v>
       </c>
@@ -1845,7 +1815,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>107</v>
       </c>
@@ -1986,34 +1956,34 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="15.69140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.3046875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.3046875" collapsed="true"/>
+    <col min="1" max="1" style="1" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.15234375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.3828125" collapsed="true"/>
-    <col min="7" max="7" style="1" width="15.69140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.3828125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.84375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.15234375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.69140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="13.3046875" collapsed="true"/>
-    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.84375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.84375" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="1" width="17.69140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" style="1" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
     <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.15234375" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.3828125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.15234375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
     <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
     <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="29" max="16384" style="1" width="15.69140625" collapsed="true"/>
+    <col min="29" max="16384" style="1" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -2099,12 +2069,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>124</v>
@@ -2135,12 +2105,12 @@
       </c>
       <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>124</v>
@@ -2170,12 +2140,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>124</v>
@@ -2205,12 +2175,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>124</v>
@@ -2250,38 +2220,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822FCC47-1993-44A8-9BE0-581A41644C90}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="15.69140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.3046875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.3046875" collapsed="true"/>
+    <col min="1" max="1" style="1" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.15234375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.3828125" collapsed="true"/>
-    <col min="7" max="7" style="1" width="15.69140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.3828125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.84375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.15234375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.69140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="13.3046875" collapsed="true"/>
-    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.84375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.84375" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="1" width="17.69140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" style="1" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
     <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.15234375" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.3828125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.15234375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
     <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
     <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="29" max="16384" style="1" width="15.69140625" collapsed="true"/>
+    <col min="29" max="16384" style="1" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -2367,12 +2337,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>124</v>
@@ -2403,12 +2373,12 @@
       </c>
       <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>124</v>
@@ -2438,12 +2408,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>124</v>
@@ -2473,12 +2443,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>124</v>
@@ -2521,34 +2491,34 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="15.69140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.3046875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.3046875" collapsed="true"/>
+    <col min="1" max="1" style="1" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.15234375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.3828125" collapsed="true"/>
-    <col min="7" max="7" style="1" width="15.69140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.3828125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.84375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.15234375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.69140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="13.3046875" collapsed="true"/>
-    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.84375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.84375" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="1" width="17.69140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" style="1" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
     <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.15234375" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.3828125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.15234375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
     <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
     <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="29" max="16384" style="1" width="15.69140625" collapsed="true"/>
+    <col min="29" max="16384" style="1" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -2634,7 +2604,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2" s="1" t="s">
@@ -2666,15 +2636,15 @@
       </c>
       <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5"/>
     </row>
@@ -2691,35 +2661,35 @@
       <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="15.69140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.3046875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.3046875" collapsed="true"/>
+    <col min="1" max="1" style="1" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.15234375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.3828125" collapsed="true"/>
-    <col min="7" max="7" style="1" width="15.69140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.3828125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.84375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="15.15234375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.69140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="13.3046875" collapsed="true"/>
-    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.84375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.84375" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="1" width="17.69140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" style="1" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="13" max="17" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
     <col min="20" max="20" customWidth="true" style="1" width="23.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.15234375" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.3828125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.15234375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
     <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
     <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" style="1" width="28.15234375" collapsed="true"/>
-    <col min="30" max="16384" style="1" width="15.69140625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="1" width="28.140625" collapsed="true"/>
+    <col min="30" max="16384" style="1" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -2808,12 +2778,12 @@
         <v>144</v>
       </c>
     </row>
-    <row ht="29.15" r="2" spans="1:29" x14ac:dyDescent="0.4">
+    <row ht="30" r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>111</v>
@@ -2850,12 +2820,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>112</v>
@@ -2891,11 +2861,11 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5"/>
     </row>
@@ -2912,49 +2882,49 @@
       <selection activeCell="AX6" sqref="AX6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="49.3828125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" style="1" width="49.42578125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="4.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="8.15234375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="8.3046875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="8.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="6.84375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="13.84375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.3828125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="5.53515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="5.5703125" collapsed="true"/>
     <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="6.15234375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.69140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="23.84375" collapsed="true"/>
-    <col min="18" max="23" bestFit="true" customWidth="true" style="1" width="9.69140625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="1" width="9.84375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="6.84375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="9.69140625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="10.69140625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="6.3828125" collapsed="true"/>
-    <col min="29" max="29" style="1" width="15.69140625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="10.3828125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="7.84375" collapsed="true"/>
-    <col min="32" max="33" bestFit="true" customWidth="true" style="1" width="9.69140625" collapsed="true"/>
-    <col min="34" max="39" bestFit="true" customWidth="true" style="1" width="7.84375" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" style="1" width="8.84375" collapsed="true"/>
-    <col min="41" max="41" customWidth="true" style="1" width="17.69140625" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="17.3046875" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="6.53515625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="8.15234375" collapsed="true"/>
-    <col min="45" max="46" bestFit="true" customWidth="true" style="1" width="7.3828125" collapsed="true"/>
-    <col min="47" max="48" bestFit="true" customWidth="true" style="1" width="9.15234375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="6.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="23.85546875" collapsed="true"/>
+    <col min="18" max="23" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="29" max="29" style="1" width="15.7109375" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="32" max="33" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="34" max="39" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="41" max="41" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="45" max="46" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="47" max="48" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
     <col min="49" max="49" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
     <col min="50" max="50" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="51" max="16384" style="1" width="15.69140625" collapsed="true"/>
+    <col min="51" max="16384" style="1" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3106,7 +3076,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>116</v>
       </c>
@@ -3153,152 +3123,152 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="56.3828125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="56.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>100</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>101</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>102</v>
       </c>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>103</v>
       </c>
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>104</v>
       </c>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>111</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>112</v>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>113</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>114</v>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>115</v>
       </c>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>120</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>121</v>
       </c>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>140</v>
       </c>
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>141</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>156</v>
       </c>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>159</v>
       </c>
@@ -3315,33 +3285,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F5F0A8-DFAA-493B-B07B-97C59CBB0D66}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.53515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.84375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.3046875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.15234375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.3828125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.69140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.3828125" collapsed="true"/>
-    <col min="9" max="17" bestFit="true" customWidth="true" width="7.84375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="8.84375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="8.53515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="17.3046875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="6.53515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="8.15234375" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" width="7.3828125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" width="6.3828125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="9" max="17" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
     <col min="27" max="27" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="8.15234375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:28" x14ac:dyDescent="0.4">
+    <row customFormat="1" r="1" s="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -3427,12 +3397,12 @@
         <v>80</v>
       </c>
     </row>
-    <row customFormat="1" ht="29.15" r="2" s="1" spans="1:28" x14ac:dyDescent="0.4">
+    <row customFormat="1" ht="45" r="2" s="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>152</v>
@@ -3444,7 +3414,7 @@
         <v>153</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>27</v>
@@ -3476,29 +3446,29 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.53515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.84375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.3046875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.15234375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.3828125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.69140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.3828125" collapsed="true"/>
-    <col min="9" max="17" bestFit="true" customWidth="true" width="7.84375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="8.84375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="8.53515625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="17.3046875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="6.53515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="8.15234375" collapsed="true"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" width="7.3828125" collapsed="true"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" width="6.3828125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="9" max="17" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="25" max="26" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
     <col min="27" max="27" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="8.15234375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:28" x14ac:dyDescent="0.4">
+    <row customFormat="1" r="1" s="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -3584,12 +3554,12 @@
         <v>80</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:28" x14ac:dyDescent="0.4">
+    <row customFormat="1" r="2" s="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>154</v>
@@ -3601,7 +3571,7 @@
         <v>153</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>27</v>

</xml_diff>